<commit_message>
update for no mpa and outside mpa
</commit_message>
<xml_diff>
--- a/data/model_list.xlsx
+++ b/data/model_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acaug\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acaug\Documents\School\PhD\mpa_climate_selection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AF1BC2-CDA4-4166-A7AB-AE53D4A55088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D29CAB-1921-4F76-AA13-2B86BE62B43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="730" windowWidth="19200" windowHeight="11270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="82">
   <si>
     <t>Model Name</t>
   </si>
@@ -241,6 +241,36 @@
   </si>
   <si>
     <t>1. No Climate - Null</t>
+  </si>
+  <si>
+    <t>Model41</t>
+  </si>
+  <si>
+    <t>Model42</t>
+  </si>
+  <si>
+    <t>Model44</t>
+  </si>
+  <si>
+    <t>Model45</t>
+  </si>
+  <si>
+    <t>Model46</t>
+  </si>
+  <si>
+    <t>Model47</t>
+  </si>
+  <si>
+    <t>Model48</t>
+  </si>
+  <si>
+    <t>Model49</t>
+  </si>
+  <si>
+    <t>Model50</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -587,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:C41"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1344,72 +1374,212 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E42" s="1"/>
+      <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E43" s="1"/>
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E44" s="1"/>
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E45" s="1"/>
+      <c r="A45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E46" s="1"/>
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E47" s="1"/>
+      <c r="A47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.35">

</xml_diff>